<commit_message>
added skill/abil rolls, updated select cases, removed perception from DB, added check mod, added some XML documentation
</commit_message>
<xml_diff>
--- a/DnD information-0.09.xlsx
+++ b/DnD information-0.09.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>pID</t>
   </si>
@@ -83,9 +83,6 @@
     <t>pHealth</t>
   </si>
   <si>
-    <t>pPerception</t>
-  </si>
-  <si>
     <t>pActionPoints</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
   </si>
   <si>
     <t>mGender</t>
-  </si>
-  <si>
-    <t>mPerception</t>
   </si>
   <si>
     <t>mActionPoints</t>
@@ -1022,7 +1016,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,17 +1034,17 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1"/>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1061,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G2"/>
     </row>
@@ -1071,14 +1065,14 @@
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3"/>
       <c r="I3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1087,10 +1081,10 @@
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G4"/>
     </row>
@@ -1100,14 +1094,14 @@
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G5"/>
       <c r="I5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1116,10 +1110,10 @@
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G6"/>
     </row>
@@ -1129,14 +1123,14 @@
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G7"/>
       <c r="I7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1145,7 +1139,7 @@
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1153,15 +1147,15 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F9" s="30"/>
       <c r="G9"/>
       <c r="I9" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1169,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G10"/>
     </row>
@@ -1178,322 +1172,316 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
+      <c r="A12" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="26" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G14"/>
       <c r="J14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
-        <v>30</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G15"/>
       <c r="J15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+        <v>31</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26" t="s">
+        <v>4</v>
+      </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26" t="s">
-        <v>4</v>
+      <c r="A17" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25" t="s">
-        <v>41</v>
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
       </c>
       <c r="G18"/>
       <c r="J18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G20"/>
       <c r="J20" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G21"/>
       <c r="J21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G22"/>
       <c r="J22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23"/>
       <c r="J23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G24"/>
       <c r="J24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G26"/>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="G27"/>
       <c r="J27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" t="s">
-        <v>122</v>
+      <c r="A28" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="28" t="s">
+        <v>68</v>
       </c>
       <c r="G28"/>
       <c r="J28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="28" t="s">
-        <v>70</v>
+      <c r="A29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G30"/>
       <c r="J30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="F37" s="30"/>
       <c r="G37"/>
     </row>
@@ -1550,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1558,7 +1546,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1566,7 +1554,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1574,7 +1562,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1582,10 +1570,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
         <v>89</v>
-      </c>
-      <c r="H5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,7 +1581,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1624,7 +1612,7 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="39" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -1634,32 +1622,32 @@
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
       <c r="K2" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="H3" s="32" t="s">
         <v>52</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>54</v>
       </c>
       <c r="I3" s="32"/>
       <c r="K3" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -1674,7 +1662,7 @@
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="K4" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1687,10 +1675,10 @@
       <c r="F5" s="7"/>
       <c r="G5" s="18"/>
       <c r="H5" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -1703,13 +1691,13 @@
       <c r="F6" s="7"/>
       <c r="G6" s="18"/>
       <c r="H6" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -1722,10 +1710,10 @@
       <c r="F7" s="7"/>
       <c r="G7" s="18"/>
       <c r="H7" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -1738,10 +1726,10 @@
       <c r="F8" s="20"/>
       <c r="G8" s="18"/>
       <c r="H8" s="24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -1758,7 +1746,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -1776,10 +1764,10 @@
       <c r="F11" s="37"/>
       <c r="G11" s="38"/>
       <c r="H11" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added powers to database and forms
</commit_message>
<xml_diff>
--- a/DnD information-0.09.xlsx
+++ b/DnD information-0.09.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
   <si>
     <t>pID</t>
   </si>
@@ -149,27 +149,6 @@
     <t>mSymbol</t>
   </si>
   <si>
-    <t>*May be unnecessary</t>
-  </si>
-  <si>
-    <t>Calculated Fields</t>
-  </si>
-  <si>
-    <t>total attack power</t>
-  </si>
-  <si>
-    <t>damage (against fortitude &amp; AC)</t>
-  </si>
-  <si>
-    <t>tot stats (taken from base stats + modifiers)</t>
-  </si>
-  <si>
-    <t>Not all mobs can be "Groc'Loc the Defecator"</t>
-  </si>
-  <si>
-    <t>mName can be NULL, pName can not</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -299,27 +278,6 @@
     <t>my character has a "Lether Helmet" (7)</t>
   </si>
   <si>
-    <t>armor bonus mod</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>light/heavy</t>
-  </si>
-  <si>
-    <t>check mod</t>
-  </si>
-  <si>
-    <t>STR, DEX, CON skill checks (not a STR check to break down a door)</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>gold pieces</t>
-  </si>
-  <si>
     <t>aWgt</t>
   </si>
   <si>
@@ -345,9 +303,6 @@
   </si>
   <si>
     <t>aType</t>
-  </si>
-  <si>
-    <t>tot weight</t>
   </si>
   <si>
     <t>aNeck</t>
@@ -507,7 +462,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -541,15 +496,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -667,22 +613,21 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -692,13 +637,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -709,25 +654,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1013,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,122 +972,114 @@
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1"/>
-      <c r="I1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="E2" s="30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3"/>
-      <c r="I3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="25" t="s">
         <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5"/>
-      <c r="I5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="25" t="s">
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25" t="s">
         <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7"/>
-      <c r="I7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1150,24 +1087,22 @@
         <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9"/>
-      <c r="I9" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="H9" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1175,114 +1110,96 @@
         <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25" t="s">
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14"/>
-      <c r="J14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
       <c r="E15" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15"/>
-      <c r="J15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25" t="s">
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24" t="s">
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="G18"/>
-      <c r="J18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1290,228 +1207,167 @@
         <v>3</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20"/>
-      <c r="J20" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21"/>
-      <c r="J21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22"/>
-      <c r="J22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23"/>
-      <c r="J23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24"/>
-      <c r="J24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
-      </c>
-      <c r="G25"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26"/>
-      <c r="J26" t="s">
-        <v>90</v>
-      </c>
-      <c r="K26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
-      </c>
-      <c r="G27"/>
-      <c r="J27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28"/>
-      <c r="J28" t="s">
-        <v>93</v>
-      </c>
-      <c r="K28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30"/>
-      <c r="J30" t="s">
-        <v>95</v>
-      </c>
-      <c r="L30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G33"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G34"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F37" s="30"/>
-      <c r="G37"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F38" s="30"/>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F39" s="30"/>
-      <c r="G39"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F40" s="30"/>
-      <c r="G40"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F41" s="30"/>
-      <c r="G41"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F42" s="30"/>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F43" s="30"/>
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F44" s="30"/>
-      <c r="G44"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="29"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" s="29"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="29"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40" s="29"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="29"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="29"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="29"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1538,7 +1394,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1546,7 +1402,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1554,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1562,7 +1418,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1570,10 +1426,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1581,7 +1437,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1611,163 +1467,163 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="K2" s="15" t="s">
+      <c r="B2" s="38" t="s">
         <v>58</v>
       </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="K2" s="14" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="31"/>
+      <c r="K3" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="K4" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="7" t="s">
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="I6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="K3" s="16" t="s">
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="K4" s="17" t="s">
+      <c r="I8" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="11" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="18" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <v>6</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>